<commit_message>
Passing adj and failing target tests
</commit_message>
<xml_diff>
--- a/data/Other/CCDF_ClueLayout.xlsx
+++ b/data/Other/CCDF_ClueLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\CSCI306\ClueGameCCDF\data\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\School\Fall 2016\Software Engineering\My Workspace\ClueGameCCDF\data\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Y35"/>
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>